<commit_message>
update to statscan data,l migration, population
</commit_message>
<xml_diff>
--- a/pop_projs.xlsx
+++ b/pop_projs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maln\Documents\GitHub\housing_stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmak\Documents\GitHub\housing_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D598FC-167A-4CE1-8E46-01BD97E80E96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="2670" windowWidth="21600" windowHeight="11835" xr2:uid="{B0D28E39-05CD-494D-BC13-5391A1DC85CE}"/>
+    <workbookView xWindow="4650" yWindow="2670" windowWidth="21600" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Year</t>
   </si>
@@ -83,11 +82,23 @@
   <si>
     <t>Non-Core</t>
   </si>
+  <si>
+    <t>Historical</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,6 +663,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -659,7 +671,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1076,6 +1087,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1083,7 +1095,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1108,6 +1119,1202 @@
         <a:defRPr>
           <a:latin typeface="Gill Sans MT" panose="020B0502020104020203" pitchFamily="34" charset="0"/>
         </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Estimated and Projected Population,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Calgary CMA</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Historical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2040</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>1002458</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1025092</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1041586</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1057949</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1083442</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1116633</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1147161</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1175318</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1207093</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1227854</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1249865</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1278541</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1316952</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1357714</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1383736</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1410240</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1436060</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1461395</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1491074</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1515555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DEEE-4205-89A3-8B1E5AEEEACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2040</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="19">
+                  <c:v>1519055</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1539095</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1561295</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1588255</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1619275</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1652995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1689370</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1729145</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1770025</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1812590</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1856320</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1901015</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1946875</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1993325</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2040500</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2088440</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2137090</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2186435</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2236485</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2287330</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2338900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DEEE-4205-89A3-8B1E5AEEEACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Med</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2040</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="19">
+                  <c:v>1515555</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1530945</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1546280</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1567775</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1592210</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1618340</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1645660</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1674735</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1704115</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1734035</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1764230</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1794550</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1825115</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1855785</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1886585</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1917560</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1948755</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1980125</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2011650</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2043405</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2075415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DEEE-4205-89A3-8B1E5AEEEACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2040</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="19">
+                  <c:v>1508510</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1521205</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1531315</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1548480</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1567905</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1588545</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1609510</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1631065</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1652465</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1673920</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1695135</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1716165</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1736985</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1757650</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1778235</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1798730</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1819140</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1839480</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1859780</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1880035</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1900325</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DEEE-4205-89A3-8B1E5AEEEACD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="7491223"/>
+        <c:axId val="7485319"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="7491223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7485319"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="7485319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7491223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1200,6 +2407,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2190,6 +3437,522 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2291,6 +4054,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>283367</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>45243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>157162</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2595,24 +4393,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF42ED52-4C8C-4B84-88BC-B747594A2CBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.86328125" customWidth="1"/>
+    <col min="8" max="8" width="15.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2650,7 +4448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2021</v>
       </c>
@@ -2692,7 +4490,7 @@
         <v>0.76752145941974448</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2030</v>
       </c>
@@ -2742,7 +4540,7 @@
         <v>1.1556637531179164</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2040</v>
       </c>
@@ -2792,7 +4590,7 @@
         <v>1.3612650730483267</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B5" s="3">
         <f>(B4/B2)-1</f>
         <v>0.36126507304832667</v>
@@ -2830,12 +4628,12 @@
         <v>0.11898933813656011</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="I9" t="s">
         <v>1</v>
       </c>
@@ -2849,7 +4647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="I10" s="1">
         <v>2273020</v>
       </c>
@@ -2865,30 +4663,500 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB864AF-82D0-40E6-B0EC-B3FE4F1C9ABE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>2001</v>
+      </c>
+      <c r="B2">
+        <v>1002458</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2002</v>
+      </c>
+      <c r="B3">
+        <v>1025092</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2003</v>
+      </c>
+      <c r="B4">
+        <v>1041586</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2004</v>
+      </c>
+      <c r="B5">
+        <v>1057949</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>2005</v>
+      </c>
+      <c r="B6">
+        <v>1083442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>2006</v>
+      </c>
+      <c r="B7">
+        <v>1116633</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>2007</v>
+      </c>
+      <c r="B8">
+        <v>1147161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>2008</v>
+      </c>
+      <c r="B9">
+        <v>1175318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>2009</v>
+      </c>
+      <c r="B10">
+        <v>1207093</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11">
+        <v>1227854</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>2011</v>
+      </c>
+      <c r="B12">
+        <v>1249865</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>2012</v>
+      </c>
+      <c r="B13">
+        <v>1278541</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>2013</v>
+      </c>
+      <c r="B14">
+        <v>1316952</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>2014</v>
+      </c>
+      <c r="B15">
+        <v>1357714</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>2015</v>
+      </c>
+      <c r="B16">
+        <v>1383736</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>2016</v>
+      </c>
+      <c r="B17">
+        <v>1410240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>2017</v>
+      </c>
+      <c r="B18">
+        <v>1436060</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2018</v>
+      </c>
+      <c r="B19">
+        <v>1461395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2019</v>
+      </c>
+      <c r="B20">
+        <v>1491074</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>2020</v>
+      </c>
+      <c r="B21">
+        <v>1515555</v>
+      </c>
+      <c r="C21">
+        <v>1519055</v>
+      </c>
+      <c r="D21">
+        <v>1515555</v>
+      </c>
+      <c r="E21">
+        <v>1508510</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>2021</v>
+      </c>
+      <c r="C22">
+        <v>1539095</v>
+      </c>
+      <c r="D22">
+        <v>1530945</v>
+      </c>
+      <c r="E22">
+        <v>1521205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>2022</v>
+      </c>
+      <c r="C23">
+        <v>1561295</v>
+      </c>
+      <c r="D23">
+        <v>1546280</v>
+      </c>
+      <c r="E23">
+        <v>1531315</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>2023</v>
+      </c>
+      <c r="C24">
+        <v>1588255</v>
+      </c>
+      <c r="D24">
+        <v>1567775</v>
+      </c>
+      <c r="E24">
+        <v>1548480</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>2024</v>
+      </c>
+      <c r="C25">
+        <v>1619275</v>
+      </c>
+      <c r="D25">
+        <v>1592210</v>
+      </c>
+      <c r="E25">
+        <v>1567905</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>2025</v>
+      </c>
+      <c r="C26">
+        <v>1652995</v>
+      </c>
+      <c r="D26">
+        <v>1618340</v>
+      </c>
+      <c r="E26">
+        <v>1588545</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>2026</v>
+      </c>
+      <c r="C27">
+        <v>1689370</v>
+      </c>
+      <c r="D27">
+        <v>1645660</v>
+      </c>
+      <c r="E27">
+        <v>1609510</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>2027</v>
+      </c>
+      <c r="C28">
+        <v>1729145</v>
+      </c>
+      <c r="D28">
+        <v>1674735</v>
+      </c>
+      <c r="E28">
+        <v>1631065</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>2028</v>
+      </c>
+      <c r="C29">
+        <v>1770025</v>
+      </c>
+      <c r="D29">
+        <v>1704115</v>
+      </c>
+      <c r="E29">
+        <v>1652465</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>2029</v>
+      </c>
+      <c r="C30">
+        <v>1812590</v>
+      </c>
+      <c r="D30">
+        <v>1734035</v>
+      </c>
+      <c r="E30">
+        <v>1673920</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>2030</v>
+      </c>
+      <c r="C31">
+        <v>1856320</v>
+      </c>
+      <c r="D31">
+        <v>1764230</v>
+      </c>
+      <c r="E31">
+        <v>1695135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>2031</v>
+      </c>
+      <c r="C32">
+        <v>1901015</v>
+      </c>
+      <c r="D32">
+        <v>1794550</v>
+      </c>
+      <c r="E32">
+        <v>1716165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>2032</v>
+      </c>
+      <c r="C33">
+        <v>1946875</v>
+      </c>
+      <c r="D33">
+        <v>1825115</v>
+      </c>
+      <c r="E33">
+        <v>1736985</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>2033</v>
+      </c>
+      <c r="C34">
+        <v>1993325</v>
+      </c>
+      <c r="D34">
+        <v>1855785</v>
+      </c>
+      <c r="E34">
+        <v>1757650</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>2034</v>
+      </c>
+      <c r="C35">
+        <v>2040500</v>
+      </c>
+      <c r="D35">
+        <v>1886585</v>
+      </c>
+      <c r="E35">
+        <v>1778235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>2035</v>
+      </c>
+      <c r="C36">
+        <v>2088440</v>
+      </c>
+      <c r="D36">
+        <v>1917560</v>
+      </c>
+      <c r="E36">
+        <v>1798730</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>2036</v>
+      </c>
+      <c r="C37">
+        <v>2137090</v>
+      </c>
+      <c r="D37">
+        <v>1948755</v>
+      </c>
+      <c r="E37">
+        <v>1819140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>2037</v>
+      </c>
+      <c r="C38">
+        <v>2186435</v>
+      </c>
+      <c r="D38">
+        <v>1980125</v>
+      </c>
+      <c r="E38">
+        <v>1839480</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>2038</v>
+      </c>
+      <c r="C39">
+        <v>2236485</v>
+      </c>
+      <c r="D39">
+        <v>2011650</v>
+      </c>
+      <c r="E39">
+        <v>1859780</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>2039</v>
+      </c>
+      <c r="C40">
+        <v>2287330</v>
+      </c>
+      <c r="D40">
+        <v>2043405</v>
+      </c>
+      <c r="E40">
+        <v>1880035</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>2040</v>
+      </c>
+      <c r="C41">
+        <v>2338900</v>
+      </c>
+      <c r="D41">
+        <v>2075415</v>
+      </c>
+      <c r="E41">
+        <v>1900325</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B1F9C2-F884-48A6-A5A5-CD1C2B4E71E8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>